<commit_message>
Modify some .md and add new module about basic operation
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlackFloat\Desktop\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lin70\Desktop\Excel-Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63D830E-1B8D-44F7-89C6-053AB035FECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CC9B56-2E0B-4F63-B105-3AA0A96863B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BAA8844-1B6E-44C4-BE00-0898D65D845C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2BAA8844-1B6E-44C4-BE00-0898D65D845C}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>機台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>size4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dutoff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -48,13 +77,26 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,9 +113,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,23 +438,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7D6A5AC-B74E-40CF-A5D9-4E467EFA0D6C}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>5</v>
       </c>
       <c r="B1">
         <v>123</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>456</v>
       </c>

</xml_diff>

<commit_message>
Update the zip example
</commit_message>
<xml_diff>
--- a/test2.xlsx
+++ b/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlackFloat\Desktop\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC11BB72-1A7D-40B7-9C67-5F18E7A96D20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8B591D-065C-45A4-A6C5-AAA6109D0C66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BAA8844-1B6E-44C4-BE00-0898D65D845C}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>

</xml_diff>